<commit_message>
CV32E40Pv2 test list update.
Signed-off-by: Pascal Gouedo <pascal.gouedo@dolphin.fr>
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/CV32E40Pv2_test_list.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/CV32E40Pv2_test_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/Vérification/CV32E40P/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-verif\cv32e40p\docs\VerifPlans\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="785" documentId="8_{FB640083-27AE-41FB-8E21-D236EBEE8ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D45474EA-5C8D-417C-83C8-74A55B935674}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEE6736-4834-4ADF-AFA4-954B8FA62B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{34FBD8F7-5E57-4B85-A296-2A419D0B8123}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{34FBD8F7-5E57-4B85-A296-2A419D0B8123}"/>
   </bookViews>
   <sheets>
     <sheet name="test_cfg" sheetId="14" r:id="rId1"/>
@@ -47,9 +47,9 @@
   <commentList>
     <comment ref="C84" authorId="0" shapeId="0" xr:uid="{C871663A-C40B-44F4-83EE-7D4E12604F17}">
       <text>
-        <t>[Commentaire à thread]
-Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
-Commentaire :
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Should be moved later in interrupt/debug regress</t>
       </text>
     </comment>
@@ -1410,7 +1410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1619,6 +1619,37 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1652,72 +1683,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="NiveauLigne_1" xfId="1" builtinId="1" iLevel="0"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="RowLevel_1" xfId="1" builtinId="1" iLevel="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -1873,7 +1842,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -2179,17 +2148,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33C417E-43DD-4FB5-8DD8-0438827DD0AC}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="68.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
         <v>263</v>
       </c>
@@ -2197,13 +2166,13 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
         <v>266</v>
       </c>
       <c r="B2" s="69"/>
     </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>170</v>
       </c>
@@ -2211,7 +2180,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>183</v>
       </c>
@@ -2219,7 +2188,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>172</v>
       </c>
@@ -2227,7 +2196,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>254</v>
       </c>
@@ -2235,7 +2204,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>164</v>
       </c>
@@ -2243,7 +2212,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>165</v>
       </c>
@@ -2251,7 +2220,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>257</v>
       </c>
@@ -2259,7 +2228,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>206</v>
       </c>
@@ -2267,7 +2236,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>177</v>
       </c>
@@ -2275,7 +2244,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>203</v>
       </c>
@@ -2283,7 +2252,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>262</v>
       </c>
@@ -2303,49 +2272,49 @@
   </sheetPr>
   <dimension ref="A1:AI285"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="91.7109375" style="54" customWidth="1"/>
-    <col min="7" max="10" width="25.7109375" style="25" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="25" customWidth="1"/>
-    <col min="13" max="13" width="29.42578125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="91.6640625" style="54" customWidth="1"/>
+    <col min="7" max="10" width="25.6640625" style="25" customWidth="1"/>
+    <col min="11" max="11" width="30.44140625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" style="25" customWidth="1"/>
     <col min="14" max="14" width="9" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="67.140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="80.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" style="3" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="67.109375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="80.33203125" style="3" customWidth="1"/>
     <col min="18" max="18" width="89" style="2" customWidth="1"/>
-    <col min="19" max="19" width="37.140625" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.109375" customWidth="1"/>
+    <col min="20" max="20" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="99" t="s">
         <v>246</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="92" t="s">
         <v>247</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="96" t="s">
         <v>245</v>
       </c>
       <c r="G1" s="26" t="s">
@@ -2375,23 +2344,23 @@
       <c r="O1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="82" t="s">
+      <c r="P1" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="Q1" s="82" t="s">
+      <c r="Q1" s="93" t="s">
         <v>238</v>
       </c>
-      <c r="R1" s="84" t="s">
+      <c r="R1" s="95" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="86"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="97"/>
       <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
@@ -2419,17 +2388,17 @@
       <c r="O2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="80"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="87"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="91"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="98"/>
       <c r="G3" s="9" t="s">
         <v>163</v>
       </c>
@@ -2457,11 +2426,11 @@
       <c r="O3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="21" t="s">
         <v>24</v>
@@ -2509,7 +2478,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="21" t="s">
         <v>24</v>
@@ -2558,7 +2527,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="21" t="s">
         <v>24</v>
@@ -2607,7 +2576,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="21" t="s">
         <v>24</v>
@@ -2656,7 +2625,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="21" t="s">
         <v>24</v>
@@ -2705,7 +2674,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="21" t="s">
         <v>24</v>
@@ -2754,7 +2723,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="21" t="s">
         <v>24</v>
@@ -2807,7 +2776,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="21" t="s">
         <v>24</v>
@@ -2860,7 +2829,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="21" t="s">
         <v>24</v>
@@ -2913,7 +2882,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="21" t="s">
         <v>24</v>
@@ -2966,7 +2935,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="21" t="s">
         <v>24</v>
@@ -3019,7 +2988,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="21" t="s">
         <v>24</v>
@@ -3070,7 +3039,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="43" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="64"/>
       <c r="B16" s="38" t="s">
         <v>24</v>
@@ -3087,7 +3056,7 @@
       <c r="F16" s="55" t="s">
         <v>198</v>
       </c>
-      <c r="G16" s="110" t="s">
+      <c r="G16" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="37" t="s">
@@ -3114,11 +3083,11 @@
       <c r="Q16" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="R16" s="111" t="s">
+      <c r="R16" s="88" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="21" t="s">
         <v>24</v>
@@ -3135,7 +3104,7 @@
       <c r="F17" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="G17" s="110" t="s">
+      <c r="G17" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="37" t="s">
@@ -3162,11 +3131,11 @@
       <c r="Q17" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="R17" s="112" t="s">
+      <c r="R17" s="89" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="21" t="s">
         <v>24</v>
@@ -3183,7 +3152,7 @@
       <c r="F18" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="G18" s="110" t="s">
+      <c r="G18" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="37" t="s">
@@ -3210,11 +3179,11 @@
       <c r="Q18" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="R18" s="112" t="s">
+      <c r="R18" s="89" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="21" t="s">
         <v>24</v>
@@ -3231,7 +3200,7 @@
       <c r="F19" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="G19" s="110" t="s">
+      <c r="G19" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H19" s="37" t="s">
@@ -3260,25 +3229,25 @@
       <c r="Q19" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="R19" s="112" t="s">
+      <c r="R19" s="89" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="93" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="D20" s="95" t="s">
+      <c r="D20" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="96" t="s">
+      <c r="E20" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="F20" s="97" t="s">
+      <c r="F20" s="54" t="s">
         <v>37</v>
       </c>
       <c r="G20" s="24"/>
@@ -3306,18 +3275,19 @@
         <f t="shared" si="0"/>
         <v>floating_pt_zfinx_instr_en</v>
       </c>
-      <c r="N20" s="98" t="s">
+      <c r="N20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O20" s="98" t="s">
+      <c r="O20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="98"/>
-      <c r="R20" s="98" t="s">
+      <c r="P20" s="2"/>
+      <c r="Q20"/>
+      <c r="R20" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="21" t="s">
         <v>24</v>
@@ -3371,7 +3341,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="21" t="s">
         <v>24</v>
@@ -3425,7 +3395,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="21" t="s">
         <v>24</v>
@@ -3474,7 +3444,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="21" t="s">
         <v>24</v>
@@ -3523,7 +3493,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="21" t="s">
         <v>24</v>
@@ -3572,7 +3542,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="21" t="s">
         <v>24</v>
@@ -3621,7 +3591,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="21" t="s">
         <v>24</v>
@@ -3670,7 +3640,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="21" t="s">
         <v>24</v>
@@ -3719,7 +3689,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="21" t="s">
         <v>24</v>
@@ -3770,7 +3740,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="21" t="s">
         <v>24</v>
@@ -3817,7 +3787,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="21" t="s">
         <v>24</v>
@@ -3866,7 +3836,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="29"/>
       <c r="B32" s="21" t="s">
         <v>24</v>
@@ -3915,7 +3885,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="11" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" s="11" customFormat="1" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="21" t="s">
         <v>24</v>
@@ -3967,7 +3937,7 @@
       </c>
       <c r="R33" s="21"/>
     </row>
-    <row r="34" spans="1:18" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
       <c r="B34" s="21" t="s">
         <v>24</v>
@@ -4018,7 +3988,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A35" s="29"/>
       <c r="B35" s="21" t="s">
         <v>24</v>
@@ -4069,7 +4039,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29"/>
       <c r="B36" s="21" t="s">
         <v>24</v>
@@ -4120,7 +4090,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="21" t="s">
         <v>24</v>
@@ -4171,7 +4141,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
       <c r="B38" s="21" t="s">
         <v>24</v>
@@ -4222,7 +4192,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29"/>
       <c r="B39" s="21" t="s">
         <v>24</v>
@@ -4273,7 +4243,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
       <c r="B40" s="21" t="s">
         <v>24</v>
@@ -4324,7 +4294,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A41" s="29"/>
       <c r="B41" s="21" t="s">
         <v>24</v>
@@ -4375,7 +4345,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="21" t="s">
         <v>24</v>
@@ -4426,7 +4396,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
       <c r="B43" s="38" t="s">
         <v>24</v>
@@ -4476,7 +4446,7 @@
       </c>
       <c r="R43" s="42"/>
     </row>
-    <row r="44" spans="1:18" s="51" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" s="51" customFormat="1" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="44" t="s">
         <v>24</v>
@@ -4534,7 +4504,7 @@
       </c>
       <c r="R44" s="50"/>
     </row>
-    <row r="45" spans="1:18" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="21" t="s">
         <v>24</v>
@@ -4585,7 +4555,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A46" s="29"/>
       <c r="B46" s="21" t="s">
         <v>24</v>
@@ -4642,7 +4612,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="47" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
       <c r="B47" s="38" t="s">
         <v>24</v>
@@ -4692,7 +4662,7 @@
       </c>
       <c r="R47" s="42"/>
     </row>
-    <row r="48" spans="1:18" s="51" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" s="51" customFormat="1" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A48" s="29"/>
       <c r="B48" s="44" t="s">
         <v>24</v>
@@ -4744,7 +4714,7 @@
       </c>
       <c r="R48" s="50"/>
     </row>
-    <row r="49" spans="1:19" s="51" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" s="51" customFormat="1" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A49" s="29"/>
       <c r="B49" s="44" t="s">
         <v>24</v>
@@ -4796,7 +4766,7 @@
       </c>
       <c r="R49" s="50"/>
     </row>
-    <row r="50" spans="1:19" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29"/>
       <c r="B50" s="21" t="s">
         <v>24</v>
@@ -4847,7 +4817,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="51" spans="1:19" s="43" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" s="43" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
       <c r="B51" s="38" t="s">
         <v>24</v>
@@ -4892,13 +4862,13 @@
       <c r="N51" s="41"/>
       <c r="O51" s="41"/>
       <c r="P51" s="60"/>
-      <c r="Q51" s="113" t="s">
+      <c r="Q51" s="90" t="s">
         <v>337</v>
       </c>
       <c r="R51" s="42"/>
       <c r="S51" s="2"/>
     </row>
-    <row r="52" spans="1:19" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="29"/>
       <c r="B52" s="21" t="s">
         <v>24</v>
@@ -4945,10 +4915,10 @@
       <c r="N52" s="17"/>
       <c r="O52" s="17"/>
       <c r="P52" s="2"/>
-      <c r="Q52" s="98"/>
+      <c r="Q52" s="2"/>
       <c r="S52" s="2"/>
     </row>
-    <row r="53" spans="1:19" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A53" s="29"/>
       <c r="B53" s="21" t="s">
         <v>24</v>
@@ -5000,7 +4970,7 @@
       </c>
       <c r="S53" s="4"/>
     </row>
-    <row r="54" spans="1:19" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A54" s="29"/>
       <c r="B54" s="21" t="s">
         <v>24</v>
@@ -5058,7 +5028,7 @@
       </c>
       <c r="S54" s="4"/>
     </row>
-    <row r="55" spans="1:19" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A55" s="29"/>
       <c r="B55" s="21" t="s">
         <v>24</v>
@@ -5116,7 +5086,7 @@
       </c>
       <c r="S55" s="4"/>
     </row>
-    <row r="56" spans="1:19" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="21" t="s">
         <v>24</v>
@@ -5174,7 +5144,7 @@
       </c>
       <c r="S56" s="4"/>
     </row>
-    <row r="57" spans="1:19" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="21" t="s">
         <v>24</v>
@@ -5225,7 +5195,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="21" t="s">
         <v>24</v>
@@ -5282,7 +5252,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="59" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8"/>
       <c r="B59" s="21" t="s">
         <v>24</v>
@@ -5329,9 +5299,9 @@
       <c r="P59" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="Q59" s="98"/>
-    </row>
-    <row r="60" spans="1:19" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q59" s="2"/>
+    </row>
+    <row r="60" spans="1:19" s="43" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="38" t="s">
         <v>24</v>
@@ -5383,7 +5353,7 @@
       </c>
       <c r="R60" s="42"/>
     </row>
-    <row r="61" spans="1:19" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="21" t="s">
         <v>24</v>
@@ -5434,7 +5404,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="21" t="s">
         <v>24</v>
@@ -5485,7 +5455,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8"/>
       <c r="B63" s="21" t="s">
         <v>24</v>
@@ -5542,7 +5512,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
       <c r="B64" s="21" t="s">
         <v>24</v>
@@ -5599,7 +5569,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="21" t="s">
         <v>24</v>
@@ -5656,7 +5626,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
       <c r="B66" s="21" t="s">
         <v>24</v>
@@ -5713,7 +5683,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="21" t="s">
         <v>24</v>
@@ -5770,7 +5740,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A68" s="8"/>
       <c r="B68" s="21" t="s">
         <v>24</v>
@@ -5833,7 +5803,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="21" t="s">
         <v>24</v>
@@ -5896,7 +5866,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="21" t="s">
         <v>24</v>
@@ -5945,7 +5915,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="21" t="s">
         <v>24</v>
@@ -5994,7 +5964,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="21" t="s">
         <v>50</v>
@@ -6032,12 +6002,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C73" s="101" t="s">
+      <c r="C73" s="33" t="s">
         <v>267</v>
       </c>
       <c r="D73" s="22" t="s">
@@ -6068,12 +6038,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C74" s="101" t="s">
+      <c r="C74" s="33" t="s">
         <v>267</v>
       </c>
       <c r="D74" s="22" t="s">
@@ -6100,12 +6070,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="101" t="s">
+      <c r="C75" s="33" t="s">
         <v>267</v>
       </c>
       <c r="D75" s="22" t="s">
@@ -6138,12 +6108,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C76" s="101" t="s">
+      <c r="C76" s="33" t="s">
         <v>267</v>
       </c>
       <c r="D76" s="22" t="s">
@@ -6176,12 +6146,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C77" s="101" t="s">
+      <c r="C77" s="33" t="s">
         <v>19</v>
       </c>
       <c r="D77" s="22" t="s">
@@ -6214,12 +6184,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C78" s="101" t="s">
+      <c r="C78" s="33" t="s">
         <v>267</v>
       </c>
       <c r="D78" s="22" t="s">
@@ -6252,12 +6222,12 @@
         <v>288</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C79" s="101" t="s">
+      <c r="C79" s="33" t="s">
         <v>19</v>
       </c>
       <c r="D79" s="22" t="s">
@@ -6283,12 +6253,12 @@
         <v>323</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C80" s="101" t="s">
+      <c r="C80" s="33" t="s">
         <v>167</v>
       </c>
       <c r="D80" s="22" t="s">
@@ -6317,12 +6287,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C81" s="101" t="s">
+      <c r="C81" s="33" t="s">
         <v>167</v>
       </c>
       <c r="D81" s="22" t="s">
@@ -6353,12 +6323,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C82" s="101" t="s">
+      <c r="C82" s="33" t="s">
         <v>167</v>
       </c>
       <c r="D82" s="22" t="s">
@@ -6384,12 +6354,12 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C83" s="101" t="s">
+      <c r="C83" s="33" t="s">
         <v>167</v>
       </c>
       <c r="D83" s="22" t="s">
@@ -6415,41 +6385,41 @@
         <v>324</v>
       </c>
     </row>
-    <row r="84" spans="1:18" s="100" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="92"/>
-      <c r="B84" s="93" t="s">
+    <row r="84" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="6"/>
+      <c r="B84" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C84" s="101" t="s">
+      <c r="C84" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="D84" s="95" t="s">
+      <c r="D84" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E84" s="96" t="s">
+      <c r="E84" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="F84" s="97" t="s">
+      <c r="F84" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G84" s="91"/>
-      <c r="H84" s="91"/>
-      <c r="I84" s="91"/>
-      <c r="J84" s="91"/>
-      <c r="K84" s="91"/>
-      <c r="L84" s="91"/>
-      <c r="M84" s="91"/>
-      <c r="N84" s="98"/>
-      <c r="O84" s="98"/>
-      <c r="P84" s="98"/>
-      <c r="Q84" s="98" t="s">
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="R84" s="99" t="s">
+      <c r="R84" s="62" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="21" t="s">
         <v>50</v>
@@ -6481,7 +6451,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="21" t="s">
         <v>50</v>
@@ -6513,12 +6483,12 @@
         <v>290</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C87" s="101" t="s">
+      <c r="C87" s="33" t="s">
         <v>18</v>
       </c>
       <c r="D87" s="22" t="s">
@@ -6544,9 +6514,9 @@
       </c>
       <c r="O87" s="17"/>
       <c r="P87" s="2"/>
-      <c r="Q87" s="98"/>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q87" s="2"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="21" t="s">
         <v>50</v>
@@ -6582,7 +6552,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="30"/>
       <c r="B89" s="21" t="s">
         <v>50</v>
@@ -6618,7 +6588,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="21" t="s">
         <v>50</v>
@@ -6654,7 +6624,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="21" t="s">
         <v>50</v>
@@ -6690,7 +6660,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="21" t="s">
         <v>50</v>
@@ -6726,7 +6696,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="93" spans="1:18" s="79" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" s="79" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="72"/>
       <c r="B93" s="73" t="s">
         <v>50</v>
@@ -6762,7 +6732,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="21" t="s">
         <v>50</v>
@@ -6796,7 +6766,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="21" t="s">
         <v>50</v>
@@ -6830,7 +6800,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="21" t="s">
         <v>50</v>
@@ -6866,7 +6836,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="21" t="s">
         <v>50</v>
@@ -6902,7 +6872,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="21" t="s">
         <v>50</v>
@@ -6938,7 +6908,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="21" t="s">
         <v>50</v>
@@ -6970,111 +6940,111 @@
         <v>278</v>
       </c>
     </row>
-    <row r="100" spans="1:19" s="100" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="92"/>
-      <c r="B100" s="93" t="s">
+    <row r="100" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="6"/>
+      <c r="B100" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C100" s="101" t="s">
+      <c r="C100" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="D100" s="95" t="s">
+      <c r="D100" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E100" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="F100" s="97" t="s">
+      <c r="F100" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="G100" s="91" t="s">
+      <c r="G100" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H100" s="91" t="s">
+      <c r="H100" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I100" s="91" t="s">
+      <c r="I100" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J100" s="91" t="s">
+      <c r="J100" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K100" s="91" t="s">
+      <c r="K100" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="L100" s="91" t="s">
+      <c r="L100" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="M100" s="91" t="s">
+      <c r="M100" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="N100" s="98" t="s">
+      <c r="N100" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O100" s="98" t="s">
+      <c r="O100" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P100" s="102" t="s">
+      <c r="P100" s="81" t="s">
         <v>273</v>
       </c>
-      <c r="Q100" s="98"/>
+      <c r="Q100" s="2"/>
       <c r="R100" s="65" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="101" spans="1:19" s="100" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="92"/>
-      <c r="B101" s="93" t="s">
+    <row r="101" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="6"/>
+      <c r="B101" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="101" t="s">
+      <c r="C101" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="D101" s="95" t="s">
+      <c r="D101" s="22" t="s">
         <v>79</v>
       </c>
       <c r="E101" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="F101" s="97" t="s">
+      <c r="F101" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="G101" s="91" t="s">
+      <c r="G101" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H101" s="91" t="s">
+      <c r="H101" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I101" s="91" t="s">
+      <c r="I101" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J101" s="91" t="s">
+      <c r="J101" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K101" s="91" t="s">
+      <c r="K101" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="L101" s="91" t="s">
+      <c r="L101" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="M101" s="91" t="s">
+      <c r="M101" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="N101" s="98" t="s">
+      <c r="N101" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O101" s="98" t="s">
+      <c r="O101" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P101" s="102" t="s">
+      <c r="P101" s="81" t="s">
         <v>273</v>
       </c>
-      <c r="Q101" s="98"/>
+      <c r="Q101" s="2"/>
       <c r="R101" s="65" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="21" t="s">
         <v>50</v>
@@ -7091,13 +7061,13 @@
       <c r="F102" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="G102" s="91"/>
-      <c r="H102" s="91"/>
-      <c r="I102" s="91"/>
-      <c r="J102" s="91"/>
-      <c r="K102" s="91"/>
-      <c r="L102" s="91"/>
-      <c r="M102" s="91"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="24"/>
+      <c r="K102" s="24"/>
+      <c r="L102" s="24"/>
+      <c r="M102" s="24"/>
       <c r="N102" s="17" t="s">
         <v>26</v>
       </c>
@@ -7110,7 +7080,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="21" t="s">
         <v>50</v>
@@ -7127,13 +7097,13 @@
       <c r="F103" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="G103" s="91"/>
-      <c r="H103" s="91"/>
-      <c r="I103" s="91"/>
-      <c r="J103" s="91"/>
-      <c r="K103" s="91"/>
-      <c r="L103" s="91"/>
-      <c r="M103" s="91"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24"/>
+      <c r="J103" s="24"/>
+      <c r="K103" s="24"/>
+      <c r="L103" s="24"/>
+      <c r="M103" s="24"/>
       <c r="N103" s="17" t="s">
         <v>26</v>
       </c>
@@ -7148,44 +7118,44 @@
         <v>280</v>
       </c>
     </row>
-    <row r="104" spans="1:19" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="92"/>
-      <c r="B104" s="93" t="s">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A104" s="6"/>
+      <c r="B104" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C104" s="94" t="s">
+      <c r="C104" s="80" t="s">
         <v>267</v>
       </c>
-      <c r="D104" s="95" t="s">
+      <c r="D104" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="E104" s="96" t="s">
+      <c r="E104" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="F104" s="97" t="s">
+      <c r="F104" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="G104" s="91"/>
-      <c r="H104" s="91"/>
-      <c r="I104" s="91"/>
-      <c r="J104" s="91"/>
-      <c r="K104" s="91"/>
-      <c r="L104" s="91"/>
-      <c r="M104" s="91"/>
-      <c r="N104" s="98" t="s">
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="24"/>
+      <c r="J104" s="24"/>
+      <c r="K104" s="24"/>
+      <c r="L104" s="24"/>
+      <c r="M104" s="24"/>
+      <c r="N104" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O104" s="98" t="s">
+      <c r="O104" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P104" s="98"/>
-      <c r="Q104" s="98"/>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
       <c r="R104" s="2" t="s">
         <v>276</v>
       </c>
       <c r="S104" s="2"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="21" t="s">
         <v>50</v>
@@ -7220,7 +7190,7 @@
       </c>
       <c r="S105" s="2"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="21" t="s">
         <v>50</v>
@@ -7255,7 +7225,7 @@
       </c>
       <c r="S106" s="4"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="21" t="s">
         <v>50</v>
@@ -7292,7 +7262,7 @@
       </c>
       <c r="S107" s="4"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
       <c r="B108" s="21" t="s">
         <v>50</v>
@@ -7327,7 +7297,7 @@
       </c>
       <c r="S108" s="4"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
       <c r="B109" s="21" t="s">
         <v>50</v>
@@ -7362,7 +7332,7 @@
       </c>
       <c r="S109" s="4"/>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
       <c r="B110" s="21" t="s">
         <v>50</v>
@@ -7396,7 +7366,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
       <c r="B111" s="21" t="s">
         <v>50</v>
@@ -7430,7 +7400,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
       <c r="B112" s="21" t="s">
         <v>50</v>
@@ -7464,7 +7434,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
       <c r="B113" s="21" t="s">
         <v>50</v>
@@ -7498,7 +7468,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="21" t="s">
         <v>50</v>
@@ -7532,7 +7502,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
       <c r="B115" s="21" t="s">
         <v>50</v>
@@ -7566,7 +7536,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
       <c r="B116" s="21" t="s">
         <v>50</v>
@@ -7600,7 +7570,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
       <c r="B117" s="21" t="s">
         <v>50</v>
@@ -7634,7 +7604,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="6"/>
       <c r="B118" s="21" t="s">
         <v>50</v>
@@ -7668,7 +7638,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" s="6"/>
       <c r="B119" s="21" t="s">
         <v>50</v>
@@ -7702,7 +7672,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
       <c r="B120" s="21" t="s">
         <v>50</v>
@@ -7736,7 +7706,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
       <c r="B121" s="21" t="s">
         <v>50</v>
@@ -7770,7 +7740,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" s="6"/>
       <c r="B122" s="21" t="s">
         <v>50</v>
@@ -7804,7 +7774,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
       <c r="B123" s="21" t="s">
         <v>50</v>
@@ -7838,7 +7808,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124" s="6"/>
       <c r="B124" s="21" t="s">
         <v>50</v>
@@ -7872,7 +7842,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" s="6"/>
       <c r="B125" s="21" t="s">
         <v>50</v>
@@ -7906,7 +7876,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
       <c r="B126" s="21" t="s">
         <v>50</v>
@@ -7940,7 +7910,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
       <c r="B127" s="21" t="s">
         <v>50</v>
@@ -7957,13 +7927,13 @@
       <c r="F127" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="G127" s="91"/>
-      <c r="H127" s="91"/>
-      <c r="I127" s="91"/>
-      <c r="J127" s="91"/>
-      <c r="K127" s="91"/>
-      <c r="L127" s="91"/>
-      <c r="M127" s="91"/>
+      <c r="G127" s="24"/>
+      <c r="H127" s="24"/>
+      <c r="I127" s="24"/>
+      <c r="J127" s="24"/>
+      <c r="K127" s="24"/>
+      <c r="L127" s="24"/>
+      <c r="M127" s="24"/>
       <c r="N127" s="17" t="s">
         <v>26</v>
       </c>
@@ -7978,7 +7948,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128" s="6"/>
       <c r="B128" s="21" t="s">
         <v>50</v>
@@ -7995,13 +7965,13 @@
       <c r="F128" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="G128" s="91"/>
-      <c r="H128" s="91"/>
-      <c r="I128" s="91"/>
-      <c r="J128" s="91"/>
-      <c r="K128" s="91"/>
-      <c r="L128" s="91"/>
-      <c r="M128" s="91"/>
+      <c r="G128" s="24"/>
+      <c r="H128" s="24"/>
+      <c r="I128" s="24"/>
+      <c r="J128" s="24"/>
+      <c r="K128" s="24"/>
+      <c r="L128" s="24"/>
+      <c r="M128" s="24"/>
       <c r="N128" s="17" t="s">
         <v>26</v>
       </c>
@@ -8014,7 +7984,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
       <c r="B129" s="21" t="s">
         <v>50</v>
@@ -8031,13 +8001,13 @@
       <c r="F129" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="G129" s="91"/>
-      <c r="H129" s="91"/>
-      <c r="I129" s="91"/>
-      <c r="J129" s="91"/>
-      <c r="K129" s="91"/>
-      <c r="L129" s="91"/>
-      <c r="M129" s="91"/>
+      <c r="G129" s="24"/>
+      <c r="H129" s="24"/>
+      <c r="I129" s="24"/>
+      <c r="J129" s="24"/>
+      <c r="K129" s="24"/>
+      <c r="L129" s="24"/>
+      <c r="M129" s="24"/>
       <c r="N129" s="17" t="s">
         <v>26</v>
       </c>
@@ -8050,7 +8020,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" s="6"/>
       <c r="B130" s="21" t="s">
         <v>50</v>
@@ -8082,7 +8052,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" s="6"/>
       <c r="B131" s="21" t="s">
         <v>50</v>
@@ -8109,10 +8079,10 @@
       <c r="N131" s="17"/>
       <c r="O131" s="17"/>
       <c r="P131" s="4"/>
-      <c r="Q131" s="114"/>
+      <c r="Q131" s="4"/>
       <c r="R131" s="4"/>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" s="6"/>
       <c r="B132" s="21" t="s">
         <v>50</v>
@@ -8139,10 +8109,10 @@
       <c r="N132" s="17"/>
       <c r="O132" s="17"/>
       <c r="P132" s="4"/>
-      <c r="Q132" s="114"/>
+      <c r="Q132" s="4"/>
       <c r="R132" s="4"/>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" s="8"/>
       <c r="B133" s="21" t="s">
         <v>50</v>
@@ -8173,9 +8143,9 @@
       </c>
       <c r="O133" s="17"/>
       <c r="P133" s="2"/>
-      <c r="Q133" s="114"/>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q133" s="4"/>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" s="8"/>
       <c r="B134" s="21" t="s">
         <v>50</v>
@@ -8212,11 +8182,11 @@
       </c>
       <c r="O134" s="17"/>
       <c r="P134" s="2"/>
-      <c r="Q134" s="114" t="s">
+      <c r="Q134" s="4" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" s="8"/>
       <c r="B135" s="21" t="s">
         <v>50</v>
@@ -8253,11 +8223,11 @@
       </c>
       <c r="O135" s="17"/>
       <c r="P135" s="2"/>
-      <c r="Q135" s="114" t="s">
+      <c r="Q135" s="4" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" s="6"/>
       <c r="B136" s="21" t="s">
         <v>50</v>
@@ -8287,7 +8257,7 @@
       <c r="Q136" s="4"/>
       <c r="R136" s="4"/>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" s="6"/>
       <c r="B137" s="21" t="s">
         <v>24</v>
@@ -8337,7 +8307,7 @@
       </c>
       <c r="R137" s="4"/>
     </row>
-    <row r="138" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="6"/>
       <c r="B138" s="21" t="s">
         <v>24</v>
@@ -8389,7 +8359,7 @@
       </c>
       <c r="R138" s="4"/>
     </row>
-    <row r="139" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="6"/>
       <c r="B139" s="21" t="s">
         <v>24</v>
@@ -8441,7 +8411,7 @@
       </c>
       <c r="R139" s="4"/>
     </row>
-    <row r="140" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="6"/>
       <c r="B140" s="21" t="s">
         <v>24</v>
@@ -8497,7 +8467,7 @@
       <c r="Q140" s="4"/>
       <c r="R140" s="4"/>
     </row>
-    <row r="141" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
       <c r="B141" s="21" t="s">
         <v>24</v>
@@ -8549,7 +8519,7 @@
       </c>
       <c r="R141" s="4"/>
     </row>
-    <row r="142" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="6"/>
       <c r="B142" s="21" t="s">
         <v>24</v>
@@ -8607,7 +8577,7 @@
       </c>
       <c r="R142" s="4"/>
     </row>
-    <row r="143" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
       <c r="B143" s="21" t="s">
         <v>24</v>
@@ -8665,7 +8635,7 @@
       </c>
       <c r="R143" s="4"/>
     </row>
-    <row r="144" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
       <c r="B144" s="21" t="s">
         <v>24</v>
@@ -8717,7 +8687,7 @@
       </c>
       <c r="R144" s="4"/>
     </row>
-    <row r="145" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="6"/>
       <c r="B145" s="21" t="s">
         <v>24</v>
@@ -8769,7 +8739,7 @@
       </c>
       <c r="R145" s="4"/>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A146" s="6"/>
       <c r="B146" s="21" t="s">
         <v>24</v>
@@ -8819,7 +8789,7 @@
       </c>
       <c r="R146" s="4"/>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
       <c r="B147" s="21" t="s">
         <v>24</v>
@@ -8871,7 +8841,7 @@
       </c>
       <c r="R147" s="4"/>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
       <c r="B148" s="21" t="s">
         <v>24</v>
@@ -8921,7 +8891,7 @@
       </c>
       <c r="R148" s="4"/>
     </row>
-    <row r="149" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="6"/>
       <c r="B149" s="21" t="s">
         <v>24</v>
@@ -8970,7 +8940,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
       <c r="B150" s="21" t="s">
         <v>24</v>
@@ -9017,7 +8987,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
       <c r="B151" s="21" t="s">
         <v>24</v>
@@ -9069,7 +9039,7 @@
       </c>
       <c r="R151" s="4"/>
     </row>
-    <row r="152" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
       <c r="B152" s="21" t="s">
         <v>24</v>
@@ -9127,7 +9097,7 @@
       </c>
       <c r="R152" s="4"/>
     </row>
-    <row r="153" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
       <c r="B153" s="21" t="s">
         <v>24</v>
@@ -9191,7 +9161,7 @@
       </c>
       <c r="R153" s="4"/>
     </row>
-    <row r="154" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
       <c r="B154" s="21" t="s">
         <v>24</v>
@@ -9255,7 +9225,7 @@
       </c>
       <c r="R154" s="4"/>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A155" s="6"/>
       <c r="C155" s="33"/>
       <c r="G155" s="37"/>
@@ -9271,7 +9241,7 @@
       <c r="Q155" s="4"/>
       <c r="R155" s="4"/>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
       <c r="C156" s="33"/>
       <c r="G156" s="37"/>
@@ -9287,7 +9257,7 @@
       <c r="Q156" s="4"/>
       <c r="R156" s="4"/>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A157" s="6"/>
       <c r="C157" s="33"/>
       <c r="G157" s="37"/>
@@ -9303,7 +9273,7 @@
       <c r="Q157" s="4"/>
       <c r="R157" s="4"/>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
       <c r="C158" s="33"/>
       <c r="G158" s="37"/>
@@ -9319,22 +9289,22 @@
       <c r="Q158" s="4"/>
       <c r="R158" s="4"/>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
-      <c r="G159" s="107"/>
-      <c r="H159" s="107"/>
-      <c r="I159" s="107"/>
-      <c r="J159" s="107"/>
-      <c r="K159" s="107"/>
-      <c r="L159" s="107"/>
-      <c r="M159" s="107"/>
-      <c r="N159" s="104"/>
-      <c r="O159" s="104"/>
-      <c r="P159" s="105"/>
-      <c r="Q159" s="105"/>
+      <c r="G159" s="13"/>
+      <c r="H159" s="13"/>
+      <c r="I159" s="13"/>
+      <c r="J159" s="13"/>
+      <c r="K159" s="13"/>
+      <c r="L159" s="13"/>
+      <c r="M159" s="13"/>
+      <c r="N159" s="83"/>
+      <c r="O159" s="83"/>
+      <c r="P159"/>
+      <c r="Q159"/>
       <c r="R159" s="4"/>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A160" s="6"/>
       <c r="G160" s="13"/>
       <c r="H160" s="13"/>
@@ -9348,29 +9318,29 @@
       <c r="Q160"/>
       <c r="R160" s="4"/>
     </row>
-    <row r="161" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="7"/>
-      <c r="B161" s="103"/>
+      <c r="B161" s="82"/>
       <c r="C161" s="35"/>
       <c r="D161" s="35"/>
       <c r="E161" s="66"/>
       <c r="F161" s="57"/>
-      <c r="G161" s="108"/>
-      <c r="H161" s="108"/>
-      <c r="I161" s="109"/>
-      <c r="J161" s="109"/>
-      <c r="K161" s="109"/>
-      <c r="L161" s="109"/>
-      <c r="M161" s="109"/>
+      <c r="G161" s="85"/>
+      <c r="H161" s="85"/>
+      <c r="I161" s="86"/>
+      <c r="J161" s="86"/>
+      <c r="K161" s="86"/>
+      <c r="L161" s="86"/>
+      <c r="M161" s="86"/>
       <c r="N161" s="15"/>
       <c r="O161" s="15"/>
       <c r="R161" s="7"/>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A162" s="8"/>
       <c r="C162" s="12"/>
       <c r="E162" s="10"/>
-      <c r="F162" s="106" t="s">
+      <c r="F162" s="84" t="s">
         <v>304</v>
       </c>
       <c r="G162" s="13"/>
@@ -9385,7 +9355,7 @@
       <c r="Q162"/>
       <c r="R162"/>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A163" s="8"/>
       <c r="C163" s="12"/>
       <c r="F163" s="32" t="s">
@@ -9429,7 +9399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A164" s="8"/>
       <c r="C164" s="11" t="s">
         <v>248</v>
@@ -9481,7 +9451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A165" s="8"/>
       <c r="E165" s="10" t="s">
         <v>159</v>
@@ -9530,7 +9500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A166" s="8"/>
       <c r="E166" s="10" t="s">
         <v>160</v>
@@ -9582,7 +9552,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A167" s="8"/>
       <c r="E167" s="10" t="s">
         <v>158</v>
@@ -9631,7 +9601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A168" s="8"/>
       <c r="C168" s="12"/>
       <c r="E168" s="10"/>
@@ -9677,7 +9647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A169" s="8"/>
       <c r="C169" s="12"/>
       <c r="F169" s="16" t="s">
@@ -9724,7 +9694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A170" s="8"/>
       <c r="C170" s="12"/>
       <c r="E170" s="10"/>
@@ -9740,7 +9710,7 @@
       <c r="Q170"/>
       <c r="R170"/>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A171" s="8"/>
       <c r="C171" s="12"/>
       <c r="E171" s="10"/>
@@ -9783,7 +9753,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A172" s="8"/>
       <c r="C172" s="12"/>
       <c r="E172" s="10"/>
@@ -9799,7 +9769,7 @@
       <c r="Q172"/>
       <c r="R172"/>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A173" s="8"/>
       <c r="C173" s="12"/>
       <c r="E173" s="10"/>
@@ -9842,7 +9812,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A174" s="8"/>
       <c r="C174" s="12"/>
       <c r="E174" s="10"/>
@@ -9858,7 +9828,7 @@
       <c r="Q174"/>
       <c r="R174"/>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A175" s="8"/>
       <c r="C175" s="12"/>
       <c r="E175" s="10"/>
@@ -9874,7 +9844,7 @@
       <c r="Q175"/>
       <c r="R175"/>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A176" s="8"/>
       <c r="C176" s="36"/>
       <c r="E176" s="13"/>
@@ -9890,7 +9860,7 @@
       <c r="Q176"/>
       <c r="R176"/>
     </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A177" s="8"/>
       <c r="C177" s="12"/>
       <c r="E177" s="10"/>
@@ -9906,7 +9876,7 @@
       <c r="Q177"/>
       <c r="R177"/>
     </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A178" s="8"/>
       <c r="C178" s="12"/>
       <c r="E178" s="10"/>
@@ -9922,7 +9892,7 @@
       <c r="Q178"/>
       <c r="R178"/>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A179" s="8"/>
       <c r="C179" s="12"/>
       <c r="E179" s="10"/>
@@ -9938,7 +9908,7 @@
       <c r="Q179"/>
       <c r="R179"/>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A180" s="8"/>
       <c r="C180" s="12"/>
       <c r="E180" s="10"/>
@@ -9954,7 +9924,7 @@
       <c r="Q180"/>
       <c r="R180"/>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A181" s="8"/>
       <c r="C181" s="12"/>
       <c r="E181" s="10"/>
@@ -9970,7 +9940,7 @@
       <c r="Q181"/>
       <c r="R181"/>
     </row>
-    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A182" s="8"/>
       <c r="C182" s="12"/>
       <c r="E182" s="10"/>
@@ -9986,7 +9956,7 @@
       <c r="Q182"/>
       <c r="R182"/>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A183" s="8"/>
       <c r="C183" s="12"/>
       <c r="E183" s="10"/>
@@ -10002,7 +9972,7 @@
       <c r="Q183"/>
       <c r="R183"/>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A184" s="8"/>
       <c r="C184" s="12"/>
       <c r="E184" s="10"/>
@@ -10018,7 +9988,7 @@
       <c r="Q184"/>
       <c r="R184"/>
     </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A185" s="8"/>
       <c r="C185" s="12"/>
       <c r="E185" s="10"/>
@@ -10034,7 +10004,7 @@
       <c r="Q185"/>
       <c r="R185"/>
     </row>
-    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A186" s="8"/>
       <c r="C186" s="12"/>
       <c r="E186" s="10"/>
@@ -10050,7 +10020,7 @@
       <c r="Q186"/>
       <c r="R186"/>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A187" s="8"/>
       <c r="C187" s="12"/>
       <c r="E187" s="10"/>
@@ -10066,7 +10036,7 @@
       <c r="Q187"/>
       <c r="R187"/>
     </row>
-    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A188" s="8"/>
       <c r="C188" s="12"/>
       <c r="E188" s="10"/>
@@ -10082,7 +10052,7 @@
       <c r="Q188"/>
       <c r="R188"/>
     </row>
-    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A189" s="8"/>
       <c r="C189" s="12"/>
       <c r="E189" s="10"/>
@@ -10098,7 +10068,7 @@
       <c r="Q189"/>
       <c r="R189"/>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A190" s="8"/>
       <c r="C190" s="12"/>
       <c r="E190" s="10"/>
@@ -10114,7 +10084,7 @@
       <c r="Q190"/>
       <c r="R190"/>
     </row>
-    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A191" s="8"/>
       <c r="C191" s="12"/>
       <c r="E191" s="10"/>
@@ -10136,7 +10106,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A192" s="8"/>
       <c r="C192" s="12"/>
       <c r="E192" s="10"/>
@@ -10158,7 +10128,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A193" s="8"/>
       <c r="C193" s="12"/>
       <c r="E193" s="10"/>
@@ -10180,7 +10150,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A194" s="8"/>
       <c r="C194" s="12"/>
       <c r="E194" s="10"/>
@@ -10202,7 +10172,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A195" s="8"/>
       <c r="C195" s="12"/>
       <c r="E195" s="10"/>
@@ -10224,7 +10194,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A196" s="8"/>
       <c r="C196" s="12"/>
       <c r="E196" s="10"/>
@@ -10246,7 +10216,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A197" s="8"/>
       <c r="C197" s="12"/>
       <c r="E197" s="10"/>
@@ -10268,7 +10238,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A198" s="8"/>
       <c r="C198" s="12"/>
       <c r="E198" s="10"/>
@@ -10290,7 +10260,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A199" s="8"/>
       <c r="C199" s="12"/>
       <c r="E199" s="10"/>
@@ -10312,7 +10282,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A200" s="8"/>
       <c r="C200" s="12"/>
       <c r="E200" s="10"/>
@@ -10334,7 +10304,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A201" s="8"/>
       <c r="C201" s="12"/>
       <c r="E201" s="10"/>
@@ -10356,7 +10326,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A202" s="8"/>
       <c r="C202" s="12"/>
       <c r="E202" s="10"/>
@@ -10378,7 +10348,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A203" s="8"/>
       <c r="C203" s="12"/>
       <c r="E203" s="10"/>
@@ -10394,7 +10364,7 @@
       <c r="Q203"/>
       <c r="R203"/>
     </row>
-    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A204" s="8"/>
       <c r="C204" s="12"/>
       <c r="E204" s="10"/>
@@ -10410,7 +10380,7 @@
       <c r="Q204"/>
       <c r="R204"/>
     </row>
-    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A205"/>
       <c r="B205" s="11"/>
       <c r="C205" s="12"/>
@@ -10427,7 +10397,7 @@
       <c r="Q205"/>
       <c r="R205"/>
     </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A206"/>
       <c r="B206" s="11"/>
       <c r="C206" s="12"/>
@@ -10444,7 +10414,7 @@
       <c r="Q206"/>
       <c r="R206"/>
     </row>
-    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A207"/>
       <c r="B207" s="11"/>
       <c r="C207" s="12"/>
@@ -10461,7 +10431,7 @@
       <c r="Q207"/>
       <c r="R207"/>
     </row>
-    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A208"/>
       <c r="B208" s="11"/>
       <c r="C208" s="12"/>
@@ -10478,7 +10448,7 @@
       <c r="Q208"/>
       <c r="R208"/>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A209"/>
       <c r="B209" s="11"/>
       <c r="C209" s="12"/>
@@ -10495,7 +10465,7 @@
       <c r="Q209"/>
       <c r="R209"/>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A210"/>
       <c r="B210" s="11"/>
       <c r="C210" s="12"/>
@@ -10512,7 +10482,7 @@
       <c r="Q210"/>
       <c r="R210"/>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A211"/>
       <c r="B211" s="11"/>
       <c r="C211" s="12"/>
@@ -10529,7 +10499,7 @@
       <c r="Q211"/>
       <c r="R211"/>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A212"/>
       <c r="B212" s="11"/>
       <c r="C212" s="12"/>
@@ -10546,7 +10516,7 @@
       <c r="Q212"/>
       <c r="R212"/>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A213"/>
       <c r="B213" s="11"/>
       <c r="C213" s="12"/>
@@ -10563,7 +10533,7 @@
       <c r="Q213"/>
       <c r="R213"/>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214"/>
       <c r="B214" s="11"/>
       <c r="C214" s="12"/>
@@ -10580,7 +10550,7 @@
       <c r="Q214"/>
       <c r="R214"/>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A215"/>
       <c r="B215" s="11"/>
       <c r="C215" s="12"/>
@@ -10597,7 +10567,7 @@
       <c r="Q215"/>
       <c r="R215"/>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A216"/>
       <c r="B216" s="11"/>
       <c r="C216" s="12"/>
@@ -10614,7 +10584,7 @@
       <c r="Q216"/>
       <c r="R216"/>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A217"/>
       <c r="B217" s="11"/>
       <c r="C217" s="12"/>
@@ -10631,7 +10601,7 @@
       <c r="Q217"/>
       <c r="R217"/>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A218"/>
       <c r="B218" s="11"/>
       <c r="C218" s="12"/>
@@ -10648,7 +10618,7 @@
       <c r="Q218"/>
       <c r="R218"/>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A219"/>
       <c r="B219" s="11"/>
       <c r="C219" s="12"/>
@@ -10665,7 +10635,7 @@
       <c r="Q219"/>
       <c r="R219"/>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A220"/>
       <c r="B220" s="11"/>
       <c r="C220" s="12"/>
@@ -10682,7 +10652,7 @@
       <c r="Q220"/>
       <c r="R220"/>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A221"/>
       <c r="B221" s="11"/>
       <c r="C221" s="12"/>
@@ -10699,7 +10669,7 @@
       <c r="Q221"/>
       <c r="R221"/>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A222"/>
       <c r="B222" s="11"/>
       <c r="C222" s="12"/>
@@ -10716,7 +10686,7 @@
       <c r="Q222"/>
       <c r="R222"/>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A223"/>
       <c r="B223" s="11"/>
       <c r="C223" s="12"/>
@@ -10733,7 +10703,7 @@
       <c r="Q223"/>
       <c r="R223"/>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A224"/>
       <c r="B224" s="11"/>
       <c r="C224" s="12"/>
@@ -10750,7 +10720,7 @@
       <c r="Q224"/>
       <c r="R224"/>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A225"/>
       <c r="B225" s="11"/>
       <c r="C225" s="12"/>
@@ -10767,7 +10737,7 @@
       <c r="Q225"/>
       <c r="R225"/>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A226"/>
       <c r="B226" s="11"/>
       <c r="C226" s="12"/>
@@ -10784,7 +10754,7 @@
       <c r="Q226"/>
       <c r="R226"/>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A227"/>
       <c r="B227" s="11"/>
       <c r="C227" s="12"/>
@@ -10801,7 +10771,7 @@
       <c r="Q227"/>
       <c r="R227"/>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A228"/>
       <c r="B228" s="11"/>
       <c r="C228" s="12"/>
@@ -10818,7 +10788,7 @@
       <c r="Q228"/>
       <c r="R228"/>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A229"/>
       <c r="B229" s="11"/>
       <c r="C229" s="12"/>
@@ -10835,7 +10805,7 @@
       <c r="Q229"/>
       <c r="R229"/>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A230"/>
       <c r="B230" s="11"/>
       <c r="C230" s="12"/>
@@ -10852,7 +10822,7 @@
       <c r="Q230"/>
       <c r="R230"/>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A231"/>
       <c r="B231" s="11"/>
       <c r="C231" s="12"/>
@@ -10869,7 +10839,7 @@
       <c r="Q231"/>
       <c r="R231"/>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A232"/>
       <c r="B232" s="11"/>
       <c r="C232" s="12"/>
@@ -10886,7 +10856,7 @@
       <c r="Q232"/>
       <c r="R232"/>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A233"/>
       <c r="B233" s="11"/>
       <c r="C233" s="12"/>
@@ -10903,7 +10873,7 @@
       <c r="Q233"/>
       <c r="R233"/>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A234"/>
       <c r="B234" s="11"/>
       <c r="C234" s="12"/>
@@ -10920,7 +10890,7 @@
       <c r="Q234"/>
       <c r="R234"/>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A235"/>
       <c r="B235" s="11"/>
       <c r="C235" s="12"/>
@@ -10937,7 +10907,7 @@
       <c r="Q235"/>
       <c r="R235"/>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A236"/>
       <c r="B236" s="11"/>
       <c r="C236" s="12"/>
@@ -10954,7 +10924,7 @@
       <c r="Q236"/>
       <c r="R236"/>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A237"/>
       <c r="B237" s="11"/>
       <c r="C237" s="12"/>
@@ -10971,7 +10941,7 @@
       <c r="Q237"/>
       <c r="R237"/>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A238"/>
       <c r="B238" s="11"/>
       <c r="C238" s="12"/>
@@ -10988,7 +10958,7 @@
       <c r="Q238"/>
       <c r="R238"/>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A239"/>
       <c r="B239" s="11"/>
       <c r="C239" s="12"/>
@@ -11005,7 +10975,7 @@
       <c r="Q239"/>
       <c r="R239"/>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A240"/>
       <c r="B240" s="11"/>
       <c r="C240" s="12"/>
@@ -11022,7 +10992,7 @@
       <c r="Q240"/>
       <c r="R240"/>
     </row>
-    <row r="241" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A241"/>
       <c r="B241" s="11"/>
       <c r="C241" s="12"/>
@@ -11039,7 +11009,7 @@
       <c r="Q241"/>
       <c r="R241"/>
     </row>
-    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A242"/>
       <c r="B242" s="11"/>
       <c r="C242" s="12"/>
@@ -11056,7 +11026,7 @@
       <c r="Q242"/>
       <c r="R242"/>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A243"/>
       <c r="B243" s="11"/>
       <c r="C243" s="12"/>
@@ -11073,7 +11043,7 @@
       <c r="Q243"/>
       <c r="R243"/>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A244"/>
       <c r="B244" s="11"/>
       <c r="C244" s="12"/>
@@ -11090,7 +11060,7 @@
       <c r="Q244"/>
       <c r="R244"/>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A245"/>
       <c r="B245" s="11"/>
       <c r="C245" s="12"/>
@@ -11107,7 +11077,7 @@
       <c r="Q245"/>
       <c r="R245"/>
     </row>
-    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A246"/>
       <c r="B246" s="11"/>
       <c r="C246" s="12"/>
@@ -11124,7 +11094,7 @@
       <c r="Q246"/>
       <c r="R246"/>
     </row>
-    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A247"/>
       <c r="B247" s="11"/>
       <c r="C247" s="12"/>
@@ -11141,7 +11111,7 @@
       <c r="Q247"/>
       <c r="R247"/>
     </row>
-    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A248"/>
       <c r="B248" s="11"/>
       <c r="C248" s="12"/>
@@ -11158,7 +11128,7 @@
       <c r="Q248"/>
       <c r="R248"/>
     </row>
-    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A249"/>
       <c r="B249" s="11"/>
       <c r="C249" s="12"/>
@@ -11175,7 +11145,7 @@
       <c r="Q249"/>
       <c r="R249"/>
     </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A250"/>
       <c r="B250" s="11"/>
       <c r="C250" s="12"/>
@@ -11192,7 +11162,7 @@
       <c r="Q250"/>
       <c r="R250"/>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A251"/>
       <c r="B251" s="11"/>
       <c r="C251" s="12"/>
@@ -11209,7 +11179,7 @@
       <c r="Q251"/>
       <c r="R251"/>
     </row>
-    <row r="252" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A252"/>
       <c r="B252" s="11"/>
       <c r="C252" s="12"/>
@@ -11226,7 +11196,7 @@
       <c r="Q252"/>
       <c r="R252"/>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A253"/>
       <c r="B253" s="11"/>
       <c r="C253" s="12"/>
@@ -11243,7 +11213,7 @@
       <c r="Q253"/>
       <c r="R253"/>
     </row>
-    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A254"/>
       <c r="B254" s="11"/>
       <c r="C254" s="12"/>
@@ -11260,7 +11230,7 @@
       <c r="Q254"/>
       <c r="R254"/>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A255"/>
       <c r="B255" s="11"/>
       <c r="C255" s="12"/>
@@ -11277,7 +11247,7 @@
       <c r="Q255"/>
       <c r="R255"/>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A256"/>
       <c r="B256" s="11"/>
       <c r="C256" s="12"/>
@@ -11294,7 +11264,7 @@
       <c r="Q256"/>
       <c r="R256"/>
     </row>
-    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257"/>
       <c r="B257" s="11"/>
       <c r="C257" s="12"/>
@@ -11311,7 +11281,7 @@
       <c r="Q257"/>
       <c r="R257"/>
     </row>
-    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258"/>
       <c r="B258" s="11"/>
       <c r="C258" s="12"/>
@@ -11328,7 +11298,7 @@
       <c r="Q258"/>
       <c r="R258"/>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259"/>
       <c r="B259" s="11"/>
       <c r="C259" s="12"/>
@@ -11345,7 +11315,7 @@
       <c r="Q259"/>
       <c r="R259"/>
     </row>
-    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260"/>
       <c r="B260" s="11"/>
       <c r="C260" s="12"/>
@@ -11362,7 +11332,7 @@
       <c r="Q260"/>
       <c r="R260"/>
     </row>
-    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261"/>
       <c r="B261" s="11"/>
       <c r="C261" s="12"/>
@@ -11379,7 +11349,7 @@
       <c r="Q261"/>
       <c r="R261"/>
     </row>
-    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262"/>
       <c r="B262" s="11"/>
       <c r="C262" s="12"/>
@@ -11396,7 +11366,7 @@
       <c r="Q262"/>
       <c r="R262"/>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263"/>
       <c r="B263" s="11"/>
       <c r="C263" s="12"/>
@@ -11413,7 +11383,7 @@
       <c r="Q263"/>
       <c r="R263"/>
     </row>
-    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264"/>
       <c r="B264" s="11"/>
       <c r="C264" s="12"/>
@@ -11430,7 +11400,7 @@
       <c r="Q264"/>
       <c r="R264"/>
     </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265"/>
       <c r="B265" s="11"/>
       <c r="C265" s="12"/>
@@ -11447,7 +11417,7 @@
       <c r="Q265"/>
       <c r="R265"/>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266"/>
       <c r="B266" s="11"/>
       <c r="C266" s="12"/>
@@ -11464,7 +11434,7 @@
       <c r="Q266"/>
       <c r="R266"/>
     </row>
-    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267"/>
       <c r="B267" s="11"/>
       <c r="C267" s="12"/>
@@ -11481,7 +11451,7 @@
       <c r="Q267"/>
       <c r="R267"/>
     </row>
-    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A268"/>
       <c r="B268" s="11"/>
       <c r="C268" s="12"/>
@@ -11498,7 +11468,7 @@
       <c r="Q268"/>
       <c r="R268"/>
     </row>
-    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A269"/>
       <c r="B269" s="11"/>
       <c r="C269" s="12"/>
@@ -11515,7 +11485,7 @@
       <c r="Q269"/>
       <c r="R269"/>
     </row>
-    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A270"/>
       <c r="B270" s="11"/>
       <c r="C270" s="12"/>
@@ -11532,7 +11502,7 @@
       <c r="Q270"/>
       <c r="R270"/>
     </row>
-    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A271"/>
       <c r="B271" s="11"/>
       <c r="C271" s="12"/>
@@ -11549,7 +11519,7 @@
       <c r="Q271"/>
       <c r="R271"/>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A272"/>
       <c r="B272" s="11"/>
       <c r="C272" s="12"/>
@@ -11566,7 +11536,7 @@
       <c r="Q272"/>
       <c r="R272"/>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A273"/>
       <c r="B273" s="11"/>
       <c r="C273" s="12"/>
@@ -11583,7 +11553,7 @@
       <c r="Q273"/>
       <c r="R273"/>
     </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A274"/>
       <c r="B274" s="11"/>
       <c r="C274" s="12"/>
@@ -11600,7 +11570,7 @@
       <c r="Q274"/>
       <c r="R274"/>
     </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A275"/>
       <c r="B275" s="11"/>
       <c r="C275" s="12"/>
@@ -11617,7 +11587,7 @@
       <c r="Q275"/>
       <c r="R275"/>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A276"/>
       <c r="B276" s="11"/>
       <c r="C276" s="12"/>
@@ -11634,7 +11604,7 @@
       <c r="Q276"/>
       <c r="R276"/>
     </row>
-    <row r="277" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A277"/>
       <c r="B277" s="11"/>
       <c r="C277" s="12"/>
@@ -11651,7 +11621,7 @@
       <c r="Q277"/>
       <c r="R277"/>
     </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A278"/>
       <c r="B278" s="11"/>
       <c r="C278" s="12"/>
@@ -11668,7 +11638,7 @@
       <c r="Q278"/>
       <c r="R278"/>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A279"/>
       <c r="B279" s="11"/>
       <c r="C279" s="12"/>
@@ -11685,7 +11655,7 @@
       <c r="Q279"/>
       <c r="R279"/>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A280"/>
       <c r="B280" s="11"/>
       <c r="C280" s="12"/>
@@ -11702,7 +11672,7 @@
       <c r="Q280"/>
       <c r="R280"/>
     </row>
-    <row r="281" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A281"/>
       <c r="B281" s="11"/>
       <c r="C281" s="12"/>
@@ -11719,7 +11689,7 @@
       <c r="Q281"/>
       <c r="R281"/>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A282"/>
       <c r="B282" s="11"/>
       <c r="C282" s="12"/>
@@ -11736,7 +11706,7 @@
       <c r="Q282"/>
       <c r="R282"/>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A283"/>
       <c r="B283" s="11"/>
       <c r="C283" s="12"/>
@@ -11753,7 +11723,7 @@
       <c r="Q283"/>
       <c r="R283"/>
     </row>
-    <row r="284" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A284"/>
       <c r="B284" s="11"/>
       <c r="C284" s="12"/>
@@ -11770,7 +11740,7 @@
       <c r="Q284"/>
       <c r="R284"/>
     </row>
-    <row r="285" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A285"/>
       <c r="B285" s="11"/>
       <c r="C285" s="12"/>
@@ -11801,17 +11771,6 @@
     <mergeCell ref="Q1:Q3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G4:Q5 N23:Q28 N20:P22 N29:P29 R16:R20 G6:M71 G72:Q99 Q145:R145 G102:Q159 N6:Q19 N30:Q71">
-    <cfRule type="containsText" dxfId="2" priority="34" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="39" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",G4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="40" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",G4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G100:O101">
     <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",G100)))</formula>
@@ -11823,15 +11782,15 @@
       <formula>NOT(ISERROR(SEARCH("yes",G100)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S104:S109">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",S104)))</formula>
+  <conditionalFormatting sqref="G4:Q5 N6:Q19 G6:M71 R16:R20 N20:P22 N23:Q28 N29:P29 N30:Q71 G72:Q99 G102:Q159 Q145:R145">
+    <cfRule type="containsText" dxfId="8" priority="34" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",S104)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="39" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",S104)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="40" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S51:S56">
@@ -11843,6 +11802,17 @@
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",S51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S104:S109">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",S104)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",S104)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",S104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -11863,26 +11833,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="254d2fc45a10493323dcacd51be5aaf4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="003ab9e0b5c5bed7880e662758cd0922" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -12131,32 +12081,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56571FB7-F663-4161-86C6-D015C0DC3932}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC83B55A-54A2-444A-971F-E1FA7680F0E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{134C5709-D691-49C9-9EA9-7BE76A18B125}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12173,4 +12118,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC83B55A-54A2-444A-971F-E1FA7680F0E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56571FB7-F663-4161-86C6-D015C0DC3932}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>